<commit_message>
feat: add compare by date
</commit_message>
<xml_diff>
--- a/queue/info/данные/мозырь.xlsx
+++ b/queue/info/данные/мозырь.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\MyDisk\WEB\CV\queue\info\данные\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0664F55B-47E5-4BC3-9184-9A7AAAB106AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5DBB0DF-6DBE-48A0-84F5-10E92A02E8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{325A99E7-3CF4-4A79-BD90-ADC3DC8BF7FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{94D5DDC5-4970-4872-86B9-4992721EE80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Мозырь" sheetId="1" r:id="rId1"/>
@@ -4591,17 +4591,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <b val="0"/>
@@ -4825,17 +4815,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24A7D880-04D9-4342-9ECD-7B01A156B016}" name="Таблица5" displayName="Таблица5" ref="A1:H405" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E856619F-20BB-422D-898B-7822A899AE87}" name="Таблица5" displayName="Таблица5" ref="A1:H405" totalsRowShown="0">
   <autoFilter ref="A1:H405" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{10EF25BE-FD3C-41DD-8819-23FD68F72009}" name="№ п.п." dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{ED4DECE6-7041-4763-AD26-CEB779CFDF31}" name="Фамилия, собственное имя, отчество (если таковое имеется) пациента" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{B1D8814F-02F8-457B-9FC8-32E383391FF8}" name="Адрес места жительства (места пребывания), телефон" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{1BBE09C0-A663-47FA-A2A2-95D7619A188B}" name="телефон" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{385774A4-BEF1-4A46-80FB-C132373E282E}" name="Пол (м,ж)" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{D23C428D-CE83-48F4-BCF6-438DBADF87BB}" name="Дата рождения" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{79DE0A7E-8992-4A34-9E43-2E811FBB273B}" name="Дата постановки на учет (число, месяц, год)" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{8D3C26BE-7014-43E4-984F-C31013A4161C}" name="диагноз" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A635C851-0C6E-4F08-B2AB-E80E656657D9}" name="№ п.п." dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{01CCDCC1-BC6E-44F8-93C1-F4B15C07E85B}" name="Фамилия, собственное имя, отчество (если таковое имеется) пациента" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C270DEC4-A33D-4469-B4F4-2FB81BAA865E}" name="Адрес места жительства (места пребывания), телефон" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{7DE3DA2B-3F04-45B9-BA87-3571333A6754}" name="телефон" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{87961610-FAF3-47BB-8A5D-F20BBD4E1403}" name="Пол (м,ж)" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{64A06A54-BB18-4552-BE86-530AF57B4B53}" name="Дата рождения" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{F45CBAB1-6A08-4E45-B4E0-FC5453E00D05}" name="Дата постановки на учет (число, месяц, год)" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{D7242520-CA01-4940-8C78-FCB06A05918C}" name="диагноз" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5137,11 +5127,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B89AD45-19E8-41B0-B424-945C9012157D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A84FDB73-1EAF-46ED-B5B4-D9BA6641770F}">
   <dimension ref="A1:H405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B405"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14428,9 +14418,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B405">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>